<commit_message>
Added Helper Package and Classes
</commit_message>
<xml_diff>
--- a/inNout Tutto.xlsx
+++ b/inNout Tutto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uzh-my.sharepoint.com/personal/remo_wiget_bf_uzh_ch/Documents/Studium HS22/SofCon/SofCon Assignment 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenny\Desktop\Programming\Java\SoftwareConstruction\tutto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A16AED0-44A3-475B-8D59-71622A6D8560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980683C5-F77D-4EC1-8658-C0E8C0183C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62759452-0326-4AC8-80CC-5F63584B3597}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{62759452-0326-4AC8-80CC-5F63584B3597}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Gameplay</t>
   </si>
@@ -141,12 +141,6 @@
   </si>
   <si>
     <t>getTopCard (pop)</t>
-  </si>
-  <si>
-    <t>Initializer</t>
-  </si>
-  <si>
-    <t>getNameFromUser()</t>
   </si>
   <si>
     <t>DiceRoller</t>
@@ -159,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,7 +195,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -217,7 +211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -515,16 +509,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1860FB0C-EBDF-48A0-9054-A1BFA5C94D7D}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -546,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -557,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -568,7 +564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -576,7 +572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -584,17 +580,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -605,12 +601,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -618,7 +614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -626,12 +622,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -639,7 +635,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -650,12 +646,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -663,7 +659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -671,7 +667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -679,7 +675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -687,7 +683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -695,28 +691,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>